<commit_message>
Classe Usuario, FormularioBeneficio e updates no blanejamento
</commit_message>
<xml_diff>
--- a/Docs/I - Planejamento/TabelaTarefas_Sprint3.xlsx
+++ b/Docs/I - Planejamento/TabelaTarefas_Sprint3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\UEL\Software_Engineer\Docs\I - Planejamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{18EB1DDF-9F80-4571-8477-273BA43382F7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EB8BFE-220A-4196-A48D-A99BA544E0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B04B963E-11FD-49DF-8DE1-BF515C305792}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
   <si>
     <t>TAREFA</t>
   </si>
@@ -111,6 +111,24 @@
   </si>
   <si>
     <t>T5, T6</t>
+  </si>
+  <si>
+    <t>Jader</t>
+  </si>
+  <si>
+    <t>Ana e Beatriz</t>
+  </si>
+  <si>
+    <t>Marco e Vinícius</t>
+  </si>
+  <si>
+    <t>gastou hoje</t>
+  </si>
+  <si>
+    <t>50min</t>
+  </si>
+  <si>
+    <t>1h</t>
   </si>
 </sst>
 </file>
@@ -474,10 +492,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE53BC35-C41F-4731-B0D1-4BD219C0FE68}">
-  <dimension ref="A1:E23"/>
+  <dimension ref="A1:F23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -487,9 +505,10 @@
     <col min="3" max="3" width="12.21875" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.88671875" customWidth="1"/>
+    <col min="6" max="6" width="12.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -505,8 +524,11 @@
       <c r="E1" s="2" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="F1" s="2" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -519,9 +541,14 @@
       <c r="D2" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="1"/>
-    </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E2" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="1" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -534,9 +561,14 @@
       <c r="D3" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E3" s="1"/>
-    </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E3" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -549,9 +581,14 @@
       <c r="D4" s="1" t="s">
         <v>7</v>
       </c>
-      <c r="E4" s="1"/>
-    </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.3">
+      <c r="E4" s="1" t="s">
+        <v>26</v>
+      </c>
+      <c r="F4" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -566,7 +603,7 @@
       </c>
       <c r="E5" s="1"/>
     </row>
-    <row r="6" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -581,7 +618,7 @@
       </c>
       <c r="E6" s="1"/>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -596,7 +633,7 @@
       </c>
       <c r="E7" s="1"/>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -611,7 +648,7 @@
       </c>
       <c r="E8" s="1"/>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -626,49 +663,49 @@
       </c>
       <c r="E9" s="1"/>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>

<commit_message>
Planejamento e Execução atualizados. Burndown, gantt e tabela pert
</commit_message>
<xml_diff>
--- a/Docs/I - Planejamento/TabelaTarefas_Sprint3.xlsx
+++ b/Docs/I - Planejamento/TabelaTarefas_Sprint3.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\marco\Desktop\UEL\Software_Engineer\Docs\I - Planejamento\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{50EB8BFE-220A-4196-A48D-A99BA544E0A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CDACF1BA-560D-40B0-8A1F-220D624832D0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="13176" xr2:uid="{B04B963E-11FD-49DF-8DE1-BF515C305792}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="36" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="47">
   <si>
     <t>TAREFA</t>
   </si>
@@ -116,19 +116,67 @@
     <t>Jader</t>
   </si>
   <si>
-    <t>Ana e Beatriz</t>
-  </si>
-  <si>
     <t>Marco e Vinícius</t>
   </si>
   <si>
     <t>gastou hoje</t>
   </si>
   <si>
-    <t>50min</t>
-  </si>
-  <si>
     <t>1h</t>
+  </si>
+  <si>
+    <t>1h + 1h + 2h</t>
+  </si>
+  <si>
+    <t>50min + 2h</t>
+  </si>
+  <si>
+    <t>Ana e Beatriz / Marco</t>
+  </si>
+  <si>
+    <t>Marco e Laís</t>
+  </si>
+  <si>
+    <t>Vinícius, Laís e Jader</t>
+  </si>
+  <si>
+    <t>Próxima Sprint</t>
+  </si>
+  <si>
+    <t xml:space="preserve">1h </t>
+  </si>
+  <si>
+    <t>0h</t>
+  </si>
+  <si>
+    <t>50min + 2h + 1h10</t>
+  </si>
+  <si>
+    <t>Ana, Beatriz e Laís</t>
+  </si>
+  <si>
+    <t>2h + 3h + 1h</t>
+  </si>
+  <si>
+    <t>3h</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 4h</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> 3h</t>
+  </si>
+  <si>
+    <t>4h</t>
+  </si>
+  <si>
+    <t>6h</t>
+  </si>
+  <si>
+    <t>1h + 2h</t>
   </si>
 </sst>
 </file>
@@ -492,10 +540,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{CE53BC35-C41F-4731-B0D1-4BD219C0FE68}">
-  <dimension ref="A1:F23"/>
+  <dimension ref="A1:G23"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="135" workbookViewId="0">
-      <selection activeCell="G10" sqref="G10"/>
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -505,10 +553,10 @@
     <col min="3" max="3" width="12.21875" customWidth="1"/>
     <col min="4" max="4" width="15.33203125" customWidth="1"/>
     <col min="5" max="5" width="19.88671875" customWidth="1"/>
-    <col min="6" max="6" width="12.109375" customWidth="1"/>
+    <col min="6" max="6" width="18" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A1" s="2" t="s">
         <v>0</v>
       </c>
@@ -525,10 +573,13 @@
         <v>18</v>
       </c>
       <c r="F1" s="2" t="s">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="2" spans="1:6" x14ac:dyDescent="0.3">
+        <v>27</v>
+      </c>
+      <c r="G1" s="2" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A2" s="1" t="s">
         <v>9</v>
       </c>
@@ -542,13 +593,16 @@
         <v>5</v>
       </c>
       <c r="E2" s="1" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="F2" s="1" t="s">
-        <v>30</v>
-      </c>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.3">
+        <v>29</v>
+      </c>
+      <c r="G2" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A3" s="1" t="s">
         <v>11</v>
       </c>
@@ -565,10 +619,13 @@
         <v>25</v>
       </c>
       <c r="F3" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6" x14ac:dyDescent="0.3">
+        <v>30</v>
+      </c>
+      <c r="G3" s="1" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A4" s="1" t="s">
         <v>8</v>
       </c>
@@ -582,13 +639,16 @@
         <v>7</v>
       </c>
       <c r="E4" s="1" t="s">
-        <v>26</v>
+        <v>31</v>
       </c>
       <c r="F4" s="1" t="s">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="5" spans="1:6" x14ac:dyDescent="0.3">
+        <v>37</v>
+      </c>
+      <c r="G4" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A5" s="1" t="s">
         <v>10</v>
       </c>
@@ -601,9 +661,17 @@
       <c r="D5" s="1" t="s">
         <v>5</v>
       </c>
-      <c r="E5" s="1"/>
-    </row>
-    <row r="6" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E5" s="1" t="s">
+        <v>25</v>
+      </c>
+      <c r="F5" s="1" t="s">
+        <v>28</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A6" s="1" t="s">
         <v>13</v>
       </c>
@@ -616,9 +684,17 @@
       <c r="D6" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="E6" s="1"/>
-    </row>
-    <row r="7" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E6" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="G6" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A7" s="1" t="s">
         <v>19</v>
       </c>
@@ -631,9 +707,17 @@
       <c r="D7" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="E7" s="1"/>
-    </row>
-    <row r="8" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E7" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="F7" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="G7" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A8" s="1" t="s">
         <v>16</v>
       </c>
@@ -646,9 +730,17 @@
       <c r="D8" s="1" t="s">
         <v>24</v>
       </c>
-      <c r="E8" s="1"/>
-    </row>
-    <row r="9" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E8" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="F8" s="1" t="s">
+        <v>35</v>
+      </c>
+      <c r="G8" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A9" s="1" t="s">
         <v>21</v>
       </c>
@@ -661,51 +753,59 @@
       <c r="D9" s="1" t="s">
         <v>20</v>
       </c>
-      <c r="E9" s="1"/>
-    </row>
-    <row r="10" spans="1:6" x14ac:dyDescent="0.3">
+      <c r="E9" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F9" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="G9" s="1" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
     </row>
-    <row r="11" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
     </row>
-    <row r="12" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
     </row>
-    <row r="13" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
     </row>
-    <row r="14" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
     </row>
-    <row r="15" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
     </row>
-    <row r="16" spans="1:6" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:7" x14ac:dyDescent="0.3">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>

</xml_diff>